<commit_message>
Update task list, timeline, and effort matrix
</commit_message>
<xml_diff>
--- a/project-management/effort-matrix.xlsx
+++ b/project-management/effort-matrix.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prest\Documents\Preston\School\University of Cincinnati\Semester 7 (Fall 2024)\CS 5001 - Senior Design I\senior-design\project-management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A15C9226-CABE-48C8-A70B-2846B7AF77A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F23C6CC4-8A40-4651-9583-0A550F36C158}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Task</t>
   </si>
@@ -44,12 +44,6 @@
   </si>
   <si>
     <t>Develop server process to receive C code, compile, and send back assembly code</t>
-  </si>
-  <si>
-    <t>Implement server process to receive C code from client</t>
-  </si>
-  <si>
-    <t>Implement server process to send assembly code to client</t>
   </si>
   <si>
     <t>Investigate current database implementation</t>
@@ -97,12 +91,6 @@
     <t>Develop basic server communication functionality</t>
   </si>
   <si>
-    <t>Implement client process to send C code to server</t>
-  </si>
-  <si>
-    <t>Implement client process to receive assembly code from server</t>
-  </si>
-  <si>
     <t>Ability for the end user to enter C code and for the code to successfully compile.</t>
   </si>
   <si>
@@ -111,12 +99,21 @@
   <si>
     <t>Ability for the program to provide a login feature that supports multiple users.</t>
   </si>
+  <si>
+    <t>Determine server implementation</t>
+  </si>
+  <si>
+    <t>Implement server process for communicating code between client and server</t>
+  </si>
+  <si>
+    <t>Determine opcode formatting and parsing operation</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -134,13 +131,31 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF1F2328"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -155,7 +170,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -169,6 +184,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -387,10 +406,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z1005"/>
+  <dimension ref="A1:Z1004"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -453,7 +472,7 @@
         <v>0.85</v>
       </c>
       <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
+      <c r="G2" s="5"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
@@ -474,12 +493,12 @@
       <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
     </row>
-    <row r="3" spans="1:26" ht="27.6" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="B3" s="3">
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="C3" s="3">
         <v>0.05</v>
@@ -488,10 +507,10 @@
         <v>0.05</v>
       </c>
       <c r="E3" s="3">
-        <v>0.8</v>
+        <v>0.1</v>
       </c>
       <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="G3" s="5"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -512,12 +531,12 @@
       <c r="Y3" s="2"/>
       <c r="Z3" s="2"/>
     </row>
-    <row r="4" spans="1:26" ht="28.8" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:26" ht="27.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="3">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="C4" s="3">
         <v>0.05</v>
@@ -526,10 +545,10 @@
         <v>0.05</v>
       </c>
       <c r="E4" s="3">
-        <v>0.65</v>
+        <v>0.8</v>
       </c>
       <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
+      <c r="G4" s="5"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
@@ -550,12 +569,12 @@
       <c r="Y4" s="2"/>
       <c r="Z4" s="2"/>
     </row>
-    <row r="5" spans="1:26" ht="31.2" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:26" ht="28.8" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" s="3">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="C5" s="3">
         <v>0.05</v>
@@ -564,10 +583,10 @@
         <v>0.05</v>
       </c>
       <c r="E5" s="3">
-        <v>0.7</v>
+        <v>0.65</v>
       </c>
       <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
+      <c r="G5" s="5"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -588,12 +607,12 @@
       <c r="Y5" s="2"/>
       <c r="Z5" s="2"/>
     </row>
-    <row r="6" spans="1:26" ht="28.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:26" ht="39.299999999999997" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="B6" s="3">
-        <v>0.2</v>
+        <v>0.7</v>
       </c>
       <c r="C6" s="3">
         <v>0.05</v>
@@ -602,10 +621,10 @@
         <v>0.05</v>
       </c>
       <c r="E6" s="3">
-        <v>0.7</v>
+        <v>0.2</v>
       </c>
       <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
+      <c r="G6" s="5"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -628,7 +647,7 @@
     </row>
     <row r="7" spans="1:26" ht="29.7" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B7" s="3">
         <v>0.05</v>
@@ -643,7 +662,7 @@
         <v>0.05</v>
       </c>
       <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
+      <c r="G7" s="5"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
@@ -666,7 +685,7 @@
     </row>
     <row r="8" spans="1:26" ht="28.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B8" s="3">
         <v>0.05</v>
@@ -681,7 +700,7 @@
         <v>0.05</v>
       </c>
       <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
+      <c r="G8" s="5"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -704,7 +723,7 @@
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B9" s="3">
         <v>0</v>
@@ -719,7 +738,7 @@
         <v>0.05</v>
       </c>
       <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
+      <c r="G9" s="5"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -742,7 +761,7 @@
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B10" s="3">
         <v>0.05</v>
@@ -757,7 +776,7 @@
         <v>0</v>
       </c>
       <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
+      <c r="G10" s="5"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
@@ -780,7 +799,7 @@
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B11" s="3">
         <v>0.1</v>
@@ -795,7 +814,7 @@
         <v>0.15</v>
       </c>
       <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
+      <c r="G11" s="5"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -818,7 +837,7 @@
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B12" s="3">
         <v>0.15</v>
@@ -833,7 +852,7 @@
         <v>0.1</v>
       </c>
       <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
+      <c r="G12" s="5"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
@@ -856,7 +875,7 @@
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B13" s="3">
         <v>0.05</v>
@@ -871,7 +890,7 @@
         <v>0.05</v>
       </c>
       <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
+      <c r="G13" s="5"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
@@ -894,7 +913,7 @@
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B14" s="3">
         <v>0.05</v>
@@ -909,7 +928,7 @@
         <v>0.05</v>
       </c>
       <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
+      <c r="G14" s="5"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
@@ -932,7 +951,7 @@
     </row>
     <row r="15" spans="1:26" ht="29.7" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B15" s="3">
         <v>0.05</v>
@@ -947,7 +966,7 @@
         <v>0</v>
       </c>
       <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
+      <c r="G15" s="5"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
@@ -968,24 +987,24 @@
       <c r="Y15" s="2"/>
       <c r="Z15" s="2"/>
     </row>
-    <row r="16" spans="1:26" ht="26.7" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:26" ht="29.7" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B16" s="3">
-        <v>0.15</v>
+        <v>0.25</v>
       </c>
       <c r="C16" s="3">
-        <v>0.7</v>
+        <v>0.25</v>
       </c>
       <c r="D16" s="3">
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
       <c r="E16" s="3">
-        <v>0.05</v>
+        <v>0.25</v>
       </c>
       <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
+      <c r="G16" s="5"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
@@ -1006,24 +1025,24 @@
       <c r="Y16" s="2"/>
       <c r="Z16" s="2"/>
     </row>
-    <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:26" ht="26.7" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B17" s="3">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="C17" s="3">
-        <v>0.75</v>
+        <v>0.7</v>
       </c>
       <c r="D17" s="3">
         <v>0.1</v>
       </c>
       <c r="E17" s="3">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
+      <c r="G17" s="5"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
@@ -1046,13 +1065,13 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B18" s="3">
-        <v>0.15</v>
+        <v>0.05</v>
       </c>
       <c r="C18" s="3">
-        <v>0.6</v>
+        <v>0.75</v>
       </c>
       <c r="D18" s="3">
         <v>0.1</v>
@@ -1061,7 +1080,7 @@
         <v>0.1</v>
       </c>
       <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
+      <c r="G18" s="5"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
@@ -1082,24 +1101,24 @@
       <c r="Y18" s="2"/>
       <c r="Z18" s="2"/>
     </row>
-    <row r="19" spans="1:26" ht="15.6" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A19" s="4" t="s">
-        <v>22</v>
+    <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A19" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="B19" s="3">
-        <v>0.95</v>
+        <v>0.15</v>
       </c>
       <c r="C19" s="3">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="D19" s="3">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="E19" s="3">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
+      <c r="G19" s="6"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
@@ -1120,24 +1139,24 @@
       <c r="Y19" s="2"/>
       <c r="Z19" s="2"/>
     </row>
-    <row r="20" spans="1:26" ht="31.8" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:26" ht="15.6" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A20" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B20" s="3">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="C20" s="3">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="D20" s="3">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="E20" s="3">
         <v>0.05</v>
       </c>
       <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
+      <c r="G20" s="5"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
@@ -1158,12 +1177,12 @@
       <c r="Y20" s="2"/>
       <c r="Z20" s="2"/>
     </row>
-    <row r="21" spans="1:26" ht="29.1" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:26" ht="31.8" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A21" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B21" s="3">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="C21" s="3">
         <v>0.05</v>
@@ -1172,10 +1191,10 @@
         <v>0.05</v>
       </c>
       <c r="E21" s="3">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
+      <c r="G21" s="5"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
@@ -1196,12 +1215,12 @@
       <c r="Y21" s="2"/>
       <c r="Z21" s="2"/>
     </row>
-    <row r="22" spans="1:26" ht="27.9" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:26" ht="29.1" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A22" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B22" s="3">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="C22" s="3">
         <v>0.05</v>
@@ -1210,10 +1229,10 @@
         <v>0.05</v>
       </c>
       <c r="E22" s="3">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
+      <c r="G22" s="5"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
@@ -1234,12 +1253,12 @@
       <c r="Y22" s="2"/>
       <c r="Z22" s="2"/>
     </row>
-    <row r="23" spans="1:26" ht="29.1" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:26" ht="28.8" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A23" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B23" s="3">
-        <v>0.7</v>
+        <v>0.1</v>
       </c>
       <c r="C23" s="3">
         <v>0.05</v>
@@ -1248,7 +1267,7 @@
         <v>0.05</v>
       </c>
       <c r="E23" s="3">
-        <v>0.2</v>
+        <v>0.8</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
@@ -1272,21 +1291,21 @@
       <c r="Y23" s="2"/>
       <c r="Z23" s="2"/>
     </row>
-    <row r="24" spans="1:26" ht="28.8" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:26" ht="42" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A24" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B24" s="3">
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
       <c r="C24" s="3">
-        <v>0.05</v>
+        <v>0.25</v>
       </c>
       <c r="D24" s="3">
-        <v>0.05</v>
+        <v>0.25</v>
       </c>
       <c r="E24" s="3">
-        <v>0.8</v>
+        <v>0.25</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
@@ -1310,21 +1329,21 @@
       <c r="Y24" s="2"/>
       <c r="Z24" s="2"/>
     </row>
-    <row r="25" spans="1:26" ht="42" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:26" ht="27.6" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A25" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B25" s="3">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="C25" s="3">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
       <c r="D25" s="3">
-        <v>0.25</v>
+        <v>0.6</v>
       </c>
       <c r="E25" s="3">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
@@ -1348,22 +1367,12 @@
       <c r="Y25" s="2"/>
       <c r="Z25" s="2"/>
     </row>
-    <row r="26" spans="1:26" ht="27.6" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A26" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B26" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="C26" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="D26" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="E26" s="3">
-        <v>0.1</v>
-      </c>
+    <row r="26" spans="1:26" ht="14.1" x14ac:dyDescent="0.4">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
@@ -28770,34 +28779,6 @@
       <c r="Y1004" s="2"/>
       <c r="Z1004" s="2"/>
     </row>
-    <row r="1005" spans="1:26" ht="14.1" x14ac:dyDescent="0.4">
-      <c r="A1005" s="2"/>
-      <c r="B1005" s="2"/>
-      <c r="C1005" s="2"/>
-      <c r="D1005" s="2"/>
-      <c r="E1005" s="2"/>
-      <c r="F1005" s="2"/>
-      <c r="G1005" s="2"/>
-      <c r="H1005" s="2"/>
-      <c r="I1005" s="2"/>
-      <c r="J1005" s="2"/>
-      <c r="K1005" s="2"/>
-      <c r="L1005" s="2"/>
-      <c r="M1005" s="2"/>
-      <c r="N1005" s="2"/>
-      <c r="O1005" s="2"/>
-      <c r="P1005" s="2"/>
-      <c r="Q1005" s="2"/>
-      <c r="R1005" s="2"/>
-      <c r="S1005" s="2"/>
-      <c r="T1005" s="2"/>
-      <c r="U1005" s="2"/>
-      <c r="V1005" s="2"/>
-      <c r="W1005" s="2"/>
-      <c r="X1005" s="2"/>
-      <c r="Y1005" s="2"/>
-      <c r="Z1005" s="2"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>